<commit_message>
Updated SEO for chocolate with peanut butter
</commit_message>
<xml_diff>
--- a/posts.xlsx
+++ b/posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sites\real_naked_swedish_chef\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D11AC2B9-ADA3-4662-8589-34006F6C9F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2972D11-5930-411B-A78F-94E39ADDDBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{DDFC909F-D7DF-4E06-93B1-17741E41654C}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Pending:</t>
-  </si>
-  <si>
-    <t>Easy Recipes Ideas | Facebook</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Recipes Taught | Facebook</t>
   </si>
@@ -39,7 +33,28 @@
     <t>Easy Recipes Group | Facebook</t>
   </si>
   <si>
-    <t>More Recipes | Facebook</t>
+    <t>Diabetic Food and Recipes | Facebook</t>
+  </si>
+  <si>
+    <t>Diabetic Support Group | Facebook</t>
+  </si>
+  <si>
+    <t>Checked and posting</t>
+  </si>
+  <si>
+    <t>Healthy food planners for diabetic people. Planeamiento de alimentacion | Facebook</t>
+  </si>
+  <si>
+    <t>Diabetic Recipes New Ideas 2024 | Facebook</t>
+  </si>
+  <si>
+    <t>DAILY DIABETIC DIET RECIPES | Facebook</t>
+  </si>
+  <si>
+    <t>Diabetes Type 2 Signs And Symptoms, Foods, Recipes, Meal, Support Group USA | Facebook</t>
+  </si>
+  <si>
+    <t>Easy Diabetic Recipes - cooking | foods | Facebook</t>
   </si>
 </sst>
 </file>
@@ -402,45 +417,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7069F1AF-4E38-43ED-A259-869A659E2137}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.facebook.com/groups/easyrecipesidea/my_pending_content" xr:uid="{41873EF9-B140-4D0D-84ED-C0155CFD42F2}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://www.facebook.com/groups/recipestaught/my_pending_content" xr:uid="{7593DB9B-B673-406C-AE03-E53423599B17}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://www.facebook.com/groups/easyrecipes105/my_pending_content" xr:uid="{2AC37C01-6DF7-4016-9194-0F666720C5B7}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://www.facebook.com/groups/220834982531478/my_pending_content" xr:uid="{BABFCBB9-1AF0-4FDB-9A73-D53CF807E33D}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.facebook.com/groups/463604924157606" xr:uid="{FAD77BA2-84CA-4C28-9C81-6CA06AAA4FBD}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.facebook.com/groups/144413888950964" xr:uid="{1BBA02B8-74DA-4A27-8EE8-ED35EF2FC85C}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://www.facebook.com/groups/197360433413" xr:uid="{8FA15571-34C2-419E-BCB5-9BF88F49BF26}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://www.facebook.com/groups/1006148591253340" xr:uid="{7AFBDF3B-C424-462D-ABC3-287FF1516C29}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://www.facebook.com/groups/652938943691405" xr:uid="{2754D181-6869-4CFD-BF5A-6172D90C728A}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://www.facebook.com/groups/easyrecipes105/" xr:uid="{76942FD6-9E5C-4EA1-870D-34FF697CEF97}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://www.facebook.com/groups/diabetestype2signsandsymptomsfoodsrecipesmeal/" xr:uid="{7FFC23C0-A052-489C-A326-E1028435D46C}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://www.facebook.com/groups/recipestaught/" xr:uid="{E5C8C49C-2F7D-4619-B0ED-67F296728631}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://www.facebook.com/groups/foods.cooking.recipes/" xr:uid="{B8C1041A-76B1-4F89-A5DD-53023C73D9D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>